<commit_message>
Done with extracting no. of github repositories
</commit_message>
<xml_diff>
--- a/GitHubRepositoryScrape/Technologies.xlsx
+++ b/GitHubRepositoryScrape/Technologies.xlsx
@@ -1,60 +1,125 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="122211"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="0" activeTab="1"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="122211"/>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <x:si>
+    <x:t>Technologies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Repository No.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Java</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+    1,467,137 repository results
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C#</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+    624,046 repository results
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kotlin</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+    97,388 repository results
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Python</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+    1,488,389 repository results
+</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-</styleSheet>
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,37 +408,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B5"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="N13" sqref="N13 N13:N13"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="16.109375" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="13.332031" style="2" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:14"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A2:B5"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="I9" sqref="I9 I9:I9"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetData>
+    <x:row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="2" t="s"/>
+      <x:c r="B2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="2" t="s"/>
+      <x:c r="B3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="2" t="s"/>
+      <x:c r="B4" s="2" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="2" t="s"/>
+      <x:c r="B5" s="2" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:9"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed activities for better understanding for others to understand
</commit_message>
<xml_diff>
--- a/GitHubRepositoryScrape/Technologies.xlsx
+++ b/GitHubRepositoryScrape/Technologies.xlsx
@@ -1,124 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <x:bookViews>
-    <x:workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="122211"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <x:si>
-    <x:t>Technologies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Repository No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Java</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-    1,467,137 repository results
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C#</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-    624,047 repository results
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kotlin</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-    97,388 repository results
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Python</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-    1,488,388 repository results
-</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Technologies</t>
+  </si>
+  <si>
+    <t>Repository No.</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Kotlin</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,68 +394,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:B5"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E13" sqref="E13 E13:E13"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:cols>
-    <x:col min="1" max="1" width="16.109375" style="2" customWidth="1"/>
-    <x:col min="2" max="2" width="13.332031" style="2" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B3" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B5" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5"/>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>